<commit_message>
filenames and class names correction for the sorting algos
</commit_message>
<xml_diff>
--- a/week1/5-Sorting/results.xlsx
+++ b/week1/5-Sorting/results.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="results" localSheetId="0">Sheet1!$A$1:$F$4</definedName>
+    <definedName name="results" localSheetId="0">Sheet1!$A$2:$F$5</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -41,6 +41,32 @@
     </textPr>
   </connection>
 </connections>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>selection</t>
+  </si>
+  <si>
+    <t>insertion</t>
+  </si>
+  <si>
+    <t>merge</t>
+  </si>
+  <si>
+    <t>quick</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>heap</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -202,7 +228,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$4</c:f>
+              <c:f>Sheet1!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -223,21 +249,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$4</c:f>
+              <c:f>Sheet1!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>2.0059319467691198E-5</c:v>
+                  <c:v>4.2611476167754799E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.8371295239776297E-4</c:v>
+                  <c:v>8.1452718668071104E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.6359765296729096E-2</c:v>
+                  <c:v>7.5940370990121603E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.8675049285284304</c:v>
+                  <c:v>7.8670451750455497</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -276,7 +302,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$4</c:f>
+              <c:f>Sheet1!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -297,21 +323,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$1:$C$4</c:f>
+              <c:f>Sheet1!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>1.2128891285101401E-5</c:v>
+                  <c:v>1.5758811410097401E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.6471332471992301E-4</c:v>
+                  <c:v>9.2170824232867604E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.103029330457502</c:v>
+                  <c:v>9.4620218767875505E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.6146016918873993</c:v>
+                  <c:v>9.4419660158097791</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -350,7 +376,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$4</c:f>
+              <c:f>Sheet1!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -371,21 +397,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$1:$D$4</c:f>
+              <c:f>Sheet1!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>4.0118638935382397E-5</c:v>
+                  <c:v>4.0384687604509001E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.6725889862718705E-4</c:v>
+                  <c:v>6.0662312667096E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.7965443861103198E-3</c:v>
+                  <c:v>7.7411589423517398E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.101537010376887</c:v>
+                  <c:v>9.9334049540454702E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -424,7 +450,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$4</c:f>
+              <c:f>Sheet1!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -445,21 +471,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$1:$E$4</c:f>
+              <c:f>Sheet1!$E$2:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0" formatCode="0.00E+00">
-                  <c:v>2.3324790163314901E-5</c:v>
+                  <c:v>2.35215931540189E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1768364351592E-4</c:v>
+                  <c:v>3.34251533138165E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1202579534219599E-3</c:v>
+                  <c:v>5.2356828647174003E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.133864703154358</c:v>
+                  <c:v>0.132511176510582</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -498,7 +524,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$4</c:f>
+              <c:f>Sheet1!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -519,21 +545,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$1:$F$4</c:f>
+              <c:f>Sheet1!$F$2:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4.7116076530073702E-5</c:v>
+                  <c:v>4.5158980603550099E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.6971808084635995E-5</c:v>
+                  <c:v>9.2227678405723697E-5</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>3.6666570304078001E-4</c:v>
+                  <c:v>4.5999766401982401E-4</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>2.8619517624974798E-3</c:v>
+                  <c:v>4.0754531307029499E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -550,11 +576,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="285680416"/>
-        <c:axId val="285680976"/>
+        <c:axId val="215117568"/>
+        <c:axId val="215118128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="285680416"/>
+        <c:axId val="215117568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -653,7 +679,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="285680976"/>
+        <c:crossAx val="215118128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -662,7 +688,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="285680976"/>
+        <c:axId val="215118128"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -775,7 +801,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="285680416"/>
+        <c:crossAx val="215117568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1403,16 +1429,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>333374</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>409574</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1701,10 +1727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1713,84 +1739,107 @@
     <col min="2" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>10</v>
       </c>
-      <c r="B1" s="1">
-        <v>2.0059319467691198E-5</v>
-      </c>
-      <c r="C1" s="1">
-        <v>1.2128891285101401E-5</v>
-      </c>
-      <c r="D1" s="1">
-        <v>4.0118638935382397E-5</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2.3324790163314901E-5</v>
-      </c>
-      <c r="F1" s="1">
-        <v>4.7116076530073702E-5</v>
+      <c r="B2" s="1">
+        <v>4.2611476167754799E-5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.5758811410097401E-5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4.0384687604509001E-5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2.35215931540189E-5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>4.5158980603550099E-5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>100</v>
       </c>
-      <c r="B2">
-        <v>7.8371295239776297E-4</v>
-      </c>
-      <c r="C2">
-        <v>9.6471332471992301E-4</v>
-      </c>
-      <c r="D2">
-        <v>5.6725889862718705E-4</v>
-      </c>
-      <c r="E2">
-        <v>3.1768364351592E-4</v>
-      </c>
-      <c r="F2" s="1">
-        <v>7.6971808084635995E-5</v>
+      <c r="B3">
+        <v>8.1452718668071104E-4</v>
+      </c>
+      <c r="C3">
+        <v>9.2170824232867604E-4</v>
+      </c>
+      <c r="D3">
+        <v>6.0662312667096E-4</v>
+      </c>
+      <c r="E3">
+        <v>3.34251533138165E-4</v>
+      </c>
+      <c r="F3" s="1">
+        <v>9.2227678405723697E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>1000</v>
       </c>
-      <c r="B3">
-        <v>7.6359765296729096E-2</v>
-      </c>
-      <c r="C3">
-        <v>0.103029330457502</v>
-      </c>
-      <c r="D3">
-        <v>7.7965443861103198E-3</v>
-      </c>
-      <c r="E3">
-        <v>5.1202579534219599E-3</v>
-      </c>
-      <c r="F3">
-        <v>3.6666570304078001E-4</v>
+      <c r="B4">
+        <v>7.5940370990121603E-2</v>
+      </c>
+      <c r="C4">
+        <v>9.4620218767875505E-2</v>
+      </c>
+      <c r="D4">
+        <v>7.7411589423517398E-3</v>
+      </c>
+      <c r="E4">
+        <v>5.2356828647174003E-3</v>
+      </c>
+      <c r="F4">
+        <v>4.5999766401982401E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>10000</v>
       </c>
-      <c r="B4">
-        <v>7.8675049285284304</v>
-      </c>
-      <c r="C4">
-        <v>9.6146016918873993</v>
-      </c>
-      <c r="D4">
-        <v>0.101537010376887</v>
-      </c>
-      <c r="E4">
-        <v>0.133864703154358</v>
-      </c>
-      <c r="F4">
-        <v>2.8619517624974798E-3</v>
+      <c r="B5">
+        <v>7.8670451750455497</v>
+      </c>
+      <c r="C5">
+        <v>9.4419660158097791</v>
+      </c>
+      <c r="D5">
+        <v>9.9334049540454702E-2</v>
+      </c>
+      <c r="E5">
+        <v>0.132511176510582</v>
+      </c>
+      <c r="F5">
+        <v>4.0754531307029499E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>